<commit_message>
Updated The Mapping Sheets to Some Point
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_To_Excel_Mapping_Sheet_Merchants.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_To_Excel_Mapping_Sheet_Merchants.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\cowpay_migration\All_Migration_Mapping_Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1037,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed a json syntax in the merchant mapping sheet
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_To_Excel_Mapping_Sheet_Merchants.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_To_Excel_Mapping_Sheet_Merchants.xlsx
@@ -403,8 +403,127 @@
     <t>AttachmentImages.PersonalIDImageUrls</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">[{"socialURL":"dasfg.gfds",
+    <t>[StatusTypeId]     ,    Settings.StatusTypeId</t>
+  </si>
+  <si>
+    <t>[Address]      ,      [OptionalAddress]</t>
+  </si>
+  <si>
+    <t>Nullable</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Parent Tag</t>
+  </si>
+  <si>
+    <t>Fullfilled Json Tag</t>
+  </si>
+  <si>
+    <t>Json Columns</t>
+  </si>
+  <si>
+    <t>Auto Generated Columns</t>
+  </si>
+  <si>
+    <t>Calculated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`id` int </t>
+  </si>
+  <si>
+    <t xml:space="preserve">`name` varchar(60) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">`country_id` int   </t>
+  </si>
+  <si>
+    <t>`created_at` timestamp</t>
+  </si>
+  <si>
+    <t>`updated_at` timestamp</t>
+  </si>
+  <si>
+    <t>`deleted_at` timestamp</t>
+  </si>
+  <si>
+    <t>CowPay Cities Table</t>
+  </si>
+  <si>
+    <t>Excel Cities Table</t>
+  </si>
+  <si>
+    <t>[Id] [smallint] IDENTITY</t>
+  </si>
+  <si>
+    <t>[CountryId] [smallint]</t>
+  </si>
+  <si>
+    <t>[Name] [nvarchar]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[CreatedDate] [datetime] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[UpdatedDate] [datetime] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[DeletedDate] [datetime] </t>
+  </si>
+  <si>
+    <t>[IsDeleted] [bit]</t>
+  </si>
+  <si>
+    <t>Cow Pay Table</t>
+  </si>
+  <si>
+    <t>`id` int unsigned NOT NULL AUTO_INCREMENT,</t>
+  </si>
+  <si>
+    <t>`name` varchar</t>
+  </si>
+  <si>
+    <t>`code` varchar</t>
+  </si>
+  <si>
+    <t>`flag` varchar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`created_at` timestamp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">`updated_at` timestamp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excel Table </t>
+  </si>
+  <si>
+    <t>[Code] [nchar](3)</t>
+  </si>
+  <si>
+    <t>[Flag] [nvarchar]</t>
+  </si>
+  <si>
+    <t>[CreatedDate] [datetime]</t>
+  </si>
+  <si>
+    <t>[UpdatedDate] [datetime]</t>
+  </si>
+  <si>
+    <t>[DeletedDate] [datetime]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  from candidate_merchants 
+  when is declined = 1 then declined 
+  when declined = 0 then Candidate,
+  Suspended ?mafeesh?
+  from users
+  case when is block = 0 and is_merchant = 1 then approved
+  when is block  = 1  and is merchant =1 then blocked </t>
+  </si>
+  <si>
+    <t>[{"socialURL":"dasfg.gfds",
   "socialType":
     {"id":"2",
     "name":"Twitter",
@@ -412,27 +531,7 @@
 ,
 {"socialURL":"dasfg.gfds",
   "socialType":
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>json Social Links (4  Lenghth Array of)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">    {"id":"2",
+    {"id":"2",
     "name":"Twitter",
     "icon":"fab fa-twitter"}}
 ,{"socialURL":"dasfg.gfds",
@@ -446,134 +545,13 @@
     "name":"Twitter",
     "icon":"fab fa-twitter"}}
 ]</t>
-    </r>
-  </si>
-  <si>
-    <t>[StatusTypeId]     ,    Settings.StatusTypeId</t>
-  </si>
-  <si>
-    <t>[Address]      ,      [OptionalAddress]</t>
-  </si>
-  <si>
-    <t>Nullable</t>
-  </si>
-  <si>
-    <t>Tag</t>
-  </si>
-  <si>
-    <t>Parent Tag</t>
-  </si>
-  <si>
-    <t>Fullfilled Json Tag</t>
-  </si>
-  <si>
-    <t>Json Columns</t>
-  </si>
-  <si>
-    <t>Auto Generated Columns</t>
-  </si>
-  <si>
-    <t>Calculated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`id` int </t>
-  </si>
-  <si>
-    <t xml:space="preserve">`name` varchar(60) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">`country_id` int   </t>
-  </si>
-  <si>
-    <t>`created_at` timestamp</t>
-  </si>
-  <si>
-    <t>`updated_at` timestamp</t>
-  </si>
-  <si>
-    <t>`deleted_at` timestamp</t>
-  </si>
-  <si>
-    <t>CowPay Cities Table</t>
-  </si>
-  <si>
-    <t>Excel Cities Table</t>
-  </si>
-  <si>
-    <t>[Id] [smallint] IDENTITY</t>
-  </si>
-  <si>
-    <t>[CountryId] [smallint]</t>
-  </si>
-  <si>
-    <t>[Name] [nvarchar]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[CreatedDate] [datetime] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[UpdatedDate] [datetime] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[DeletedDate] [datetime] </t>
-  </si>
-  <si>
-    <t>[IsDeleted] [bit]</t>
-  </si>
-  <si>
-    <t>Cow Pay Table</t>
-  </si>
-  <si>
-    <t>`id` int unsigned NOT NULL AUTO_INCREMENT,</t>
-  </si>
-  <si>
-    <t>`name` varchar</t>
-  </si>
-  <si>
-    <t>`code` varchar</t>
-  </si>
-  <si>
-    <t>`flag` varchar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`created_at` timestamp </t>
-  </si>
-  <si>
-    <t xml:space="preserve">`updated_at` timestamp </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Excel Table </t>
-  </si>
-  <si>
-    <t>[Code] [nchar](3)</t>
-  </si>
-  <si>
-    <t>[Flag] [nvarchar]</t>
-  </si>
-  <si>
-    <t>[CreatedDate] [datetime]</t>
-  </si>
-  <si>
-    <t>[UpdatedDate] [datetime]</t>
-  </si>
-  <si>
-    <t>[DeletedDate] [datetime]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  from candidate_merchants 
-  when is declined = 1 then declined 
-  when declined = 0 then Candidate,
-  Suspended ?mafeesh?
-  from users
-  case when is block = 0 and is_merchant = 1 then approved
-  when is block  = 1  and is merchant =1 then blocked </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -602,13 +580,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1037,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1235,7 +1206,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>116</v>
@@ -1337,7 +1308,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>110</v>
@@ -1615,52 +1586,52 @@
     </row>
     <row r="67" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="19"/>
       <c r="B73" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="15"/>
       <c r="B75" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="14"/>
       <c r="B76" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="11"/>
       <c r="B77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="12"/>
       <c r="B78" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="17"/>
       <c r="B79" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1689,63 +1660,63 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" t="s">
         <v>141</v>
-      </c>
-      <c r="C1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1769,71 +1740,71 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
H - Finished the WithdrawalRequestsTransactions
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_To_Excel_Mapping_Sheet_Merchants.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_To_Excel_Mapping_Sheet_Merchants.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="166">
   <si>
     <t xml:space="preserve">Source Table Columns </t>
   </si>
@@ -545,6 +545,12 @@
     "name":"Twitter",
     "icon":"fab fa-twitter"}}
 ]</t>
+  </si>
+  <si>
+    <t>old_id = id</t>
+  </si>
+  <si>
+    <t>old_code=m_code</t>
   </si>
 </sst>
 </file>
@@ -585,7 +591,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -658,6 +664,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -680,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -726,6 +738,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1008,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1345,6 +1358,9 @@
       <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="C28" s="23" t="s">
+        <v>164</v>
+      </c>
       <c r="E28" t="s">
         <v>113</v>
       </c>
@@ -1352,6 +1368,9 @@
     <row r="29" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>28</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">

</xml_diff>